<commit_message>
Split track to separate splines. AI data - wip
Split track to separate splines. AI data - wip
</commit_message>
<xml_diff>
--- a/Assets/Sources/Tracks/level_1.xlsx
+++ b/Assets/Sources/Tracks/level_1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="38">
   <si>
     <t>M</t>
   </si>
@@ -118,6 +118,18 @@
   </si>
   <si>
     <t>LD</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
 </sst>
 </file>
@@ -545,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="A403" workbookViewId="0">
+      <selection activeCell="D439" sqref="D439"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,7 +978,9 @@
       <c r="B33" s="6">
         <v>1</v>
       </c>
-      <c r="C33" s="6"/>
+      <c r="C33" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="D33" s="7"/>
       <c r="E33" s="3"/>
     </row>
@@ -986,8 +1000,8 @@
       <c r="B35" s="6">
         <v>3</v>
       </c>
-      <c r="C35" s="6">
-        <v>11</v>
+      <c r="C35" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="3"/>
@@ -997,8 +1011,8 @@
       <c r="B36" s="6">
         <v>2</v>
       </c>
-      <c r="C36" s="6">
-        <v>11</v>
+      <c r="C36" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="3"/>
@@ -1017,7 +1031,9 @@
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
+      <c r="C38" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="D38" s="7"/>
       <c r="E38" s="3"/>
     </row>
@@ -1549,30 +1565,34 @@
       <c r="E99" s="3"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="6"/>
+      <c r="A100" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="B100" s="6"/>
       <c r="C100" s="6"/>
-      <c r="D100" s="7"/>
+      <c r="D100" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="E100" s="3"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="6">
-        <v>32</v>
-      </c>
-      <c r="B101" s="6">
-        <v>11</v>
-      </c>
-      <c r="C101" s="6">
-        <v>11</v>
-      </c>
-      <c r="D101" s="7">
-        <v>32</v>
+      <c r="A101" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="E101" s="3"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="6">
-        <v>11</v>
+      <c r="A102" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="B102" s="6">
         <v>1</v>
@@ -1580,14 +1600,14 @@
       <c r="C102" s="6">
         <v>1</v>
       </c>
-      <c r="D102" s="7">
-        <v>11</v>
+      <c r="D102" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="E102" s="3"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="6">
-        <v>11</v>
+      <c r="A103" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="B103" s="6">
         <v>1</v>
@@ -1595,24 +1615,30 @@
       <c r="C103" s="6">
         <v>1</v>
       </c>
-      <c r="D103" s="7">
-        <v>11</v>
+      <c r="D103" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="E103" s="3"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="6"/>
+      <c r="A104" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="B104" s="6">
         <v>1</v>
       </c>
       <c r="C104" s="6">
         <v>1</v>
       </c>
-      <c r="D104" s="7"/>
+      <c r="D104" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="E104" s="3"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="6"/>
+      <c r="A105" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="B105" s="6">
         <v>1</v>
       </c>
@@ -2261,7 +2287,9 @@
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="6"/>
       <c r="B174" s="6"/>
-      <c r="C174" s="6"/>
+      <c r="C174" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="D174" s="7"/>
       <c r="E174" s="3"/>
     </row>
@@ -2279,8 +2307,8 @@
       <c r="B176" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C176" s="6">
-        <v>11</v>
+      <c r="C176" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="D176" s="7" t="s">
         <v>6</v>
@@ -2298,7 +2326,9 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="6"/>
-      <c r="B178" s="6"/>
+      <c r="B178" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C178" s="6"/>
       <c r="D178" s="7"/>
       <c r="E178" s="3"/>
@@ -2316,8 +2346,8 @@
       <c r="A180" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B180" s="6">
-        <v>11</v>
+      <c r="B180" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="C180" s="6" t="s">
         <v>2</v>
@@ -2359,8 +2389,8 @@
       <c r="B184" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C184" s="6">
-        <v>11</v>
+      <c r="C184" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="D184" s="7" t="s">
         <v>6</v>
@@ -2381,7 +2411,9 @@
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="6"/>
       <c r="B186" s="6"/>
-      <c r="C186" s="6"/>
+      <c r="C186" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="D186" s="7"/>
       <c r="E186" s="3"/>
     </row>
@@ -2444,9 +2476,13 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="6"/>
-      <c r="B194" s="6"/>
+      <c r="B194" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C194" s="6"/>
-      <c r="D194" s="7"/>
+      <c r="D194" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="E194" s="3"/>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -2462,44 +2498,52 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="6"/>
-      <c r="B196" s="6">
-        <v>11</v>
+      <c r="B196" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="C196" s="6"/>
-      <c r="D196" s="7">
-        <v>11</v>
+      <c r="D196" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="E196" s="3"/>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A197" s="6"/>
-      <c r="B197" s="6">
-        <v>11</v>
-      </c>
-      <c r="C197" s="6"/>
-      <c r="D197" s="7">
-        <v>11</v>
+      <c r="A197" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B197" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C197" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D197" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="E197" s="3"/>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A198" s="6">
-        <v>11</v>
-      </c>
-      <c r="B198" s="6"/>
-      <c r="C198" s="6">
-        <v>11</v>
-      </c>
-      <c r="D198" s="7"/>
+      <c r="A198" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B198" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C198" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D198" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="E198" s="3"/>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A199" s="6">
-        <v>11</v>
+      <c r="A199" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="B199" s="6"/>
-      <c r="C199" s="6">
-        <v>11</v>
+      <c r="C199" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="D199" s="7"/>
       <c r="E199" s="3"/>
@@ -2516,9 +2560,13 @@
       <c r="E200" s="3"/>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A201" s="6"/>
+      <c r="A201" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="B201" s="6"/>
-      <c r="C201" s="6"/>
+      <c r="C201" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="D201" s="7"/>
       <c r="E201" s="3"/>
     </row>
@@ -4731,13 +4779,13 @@
       <c r="E439" s="3"/>
     </row>
     <row r="440" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A440" s="6">
-        <v>1</v>
+      <c r="A440" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="B440" s="6"/>
       <c r="C440" s="6"/>
-      <c r="D440" s="7">
-        <v>1</v>
+      <c r="D440" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="E440" s="3"/>
     </row>

</xml_diff>

<commit_message>
Add deathloop, correct AI, change some links to Locator
</commit_message>
<xml_diff>
--- a/Assets/Sources/Tracks/level_1.xlsx
+++ b/Assets/Sources/Tracks/level_1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="42">
   <si>
     <t>M</t>
   </si>
@@ -130,6 +130,18 @@
   </si>
   <si>
     <t>11</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>shift left</t>
+  </si>
+  <si>
+    <t>shift right</t>
   </si>
 </sst>
 </file>
@@ -557,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A403" workbookViewId="0">
-      <selection activeCell="D439" sqref="D439"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,8 +718,12 @@
       <c r="J6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -732,8 +748,12 @@
       <c r="J7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="K7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1968,105 +1988,135 @@
         <v>14</v>
       </c>
       <c r="D137" s="7"/>
-      <c r="E137" s="3"/>
+      <c r="E137" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="6"/>
       <c r="B138" s="6"/>
       <c r="C138" s="6"/>
       <c r="D138" s="7"/>
-      <c r="E138" s="3"/>
+      <c r="E138" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="6"/>
       <c r="B139" s="6"/>
       <c r="C139" s="6"/>
       <c r="D139" s="7"/>
-      <c r="E139" s="3"/>
+      <c r="E139" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="6"/>
       <c r="B140" s="6"/>
       <c r="C140" s="6"/>
       <c r="D140" s="7"/>
-      <c r="E140" s="3"/>
+      <c r="E140" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="6"/>
       <c r="B141" s="6"/>
       <c r="C141" s="6"/>
       <c r="D141" s="7"/>
-      <c r="E141" s="3"/>
+      <c r="E141" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="6"/>
       <c r="B142" s="6"/>
       <c r="C142" s="6"/>
       <c r="D142" s="7"/>
-      <c r="E142" s="3"/>
+      <c r="E142" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="6"/>
       <c r="B143" s="6"/>
       <c r="C143" s="6"/>
       <c r="D143" s="7"/>
-      <c r="E143" s="3"/>
+      <c r="E143" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="6"/>
       <c r="B144" s="6"/>
       <c r="C144" s="6"/>
       <c r="D144" s="7"/>
-      <c r="E144" s="3"/>
+      <c r="E144" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="6"/>
       <c r="B145" s="6"/>
       <c r="C145" s="6"/>
       <c r="D145" s="7"/>
-      <c r="E145" s="3"/>
+      <c r="E145" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="6"/>
       <c r="B146" s="6"/>
       <c r="C146" s="6"/>
       <c r="D146" s="7"/>
-      <c r="E146" s="3"/>
+      <c r="E146" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="6"/>
       <c r="B147" s="6"/>
       <c r="C147" s="6"/>
       <c r="D147" s="7"/>
-      <c r="E147" s="3"/>
+      <c r="E147" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="6"/>
       <c r="B148" s="6"/>
       <c r="C148" s="6"/>
       <c r="D148" s="7"/>
-      <c r="E148" s="3"/>
+      <c r="E148" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="6"/>
       <c r="B149" s="6"/>
       <c r="C149" s="6"/>
       <c r="D149" s="7"/>
-      <c r="E149" s="3"/>
+      <c r="E149" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="6"/>
       <c r="B150" s="6"/>
       <c r="C150" s="6"/>
       <c r="D150" s="7"/>
-      <c r="E150" s="3"/>
+      <c r="E150" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="6"/>
       <c r="B151" s="6"/>
       <c r="C151" s="6"/>
       <c r="D151" s="7"/>
-      <c r="E151" s="3"/>
+      <c r="E151" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="6"/>
@@ -2077,84 +2127,108 @@
         <v>6</v>
       </c>
       <c r="D152" s="7"/>
-      <c r="E152" s="3"/>
+      <c r="E152" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="6"/>
       <c r="B153" s="6"/>
       <c r="C153" s="6"/>
       <c r="D153" s="7"/>
-      <c r="E153" s="3"/>
+      <c r="E153" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="6"/>
       <c r="B154" s="6"/>
       <c r="C154" s="6"/>
       <c r="D154" s="7"/>
-      <c r="E154" s="3"/>
+      <c r="E154" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="6"/>
       <c r="B155" s="6"/>
       <c r="C155" s="6"/>
       <c r="D155" s="7"/>
-      <c r="E155" s="3"/>
+      <c r="E155" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="6"/>
       <c r="B156" s="6"/>
       <c r="C156" s="6"/>
       <c r="D156" s="7"/>
-      <c r="E156" s="3"/>
+      <c r="E156" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="6"/>
       <c r="B157" s="6"/>
       <c r="C157" s="6"/>
       <c r="D157" s="7"/>
-      <c r="E157" s="3"/>
+      <c r="E157" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="6"/>
       <c r="B158" s="6"/>
       <c r="C158" s="6"/>
       <c r="D158" s="7"/>
-      <c r="E158" s="3"/>
+      <c r="E158" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="6"/>
       <c r="B159" s="6"/>
       <c r="C159" s="6"/>
       <c r="D159" s="7"/>
-      <c r="E159" s="3"/>
+      <c r="E159" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="6"/>
       <c r="B160" s="6"/>
       <c r="C160" s="6"/>
       <c r="D160" s="7"/>
-      <c r="E160" s="3"/>
+      <c r="E160" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="6"/>
       <c r="B161" s="6"/>
       <c r="C161" s="6"/>
       <c r="D161" s="7"/>
-      <c r="E161" s="3"/>
+      <c r="E161" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="6"/>
       <c r="B162" s="6"/>
       <c r="C162" s="6"/>
       <c r="D162" s="7"/>
-      <c r="E162" s="3"/>
+      <c r="E162" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="6"/>
       <c r="B163" s="6"/>
       <c r="C163" s="6"/>
       <c r="D163" s="7"/>
-      <c r="E163" s="3"/>
+      <c r="E163" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="6" t="s">
@@ -2169,7 +2243,7 @@
       <c r="D164" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E164" s="3" t="s">
+      <c r="E164" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2186,7 +2260,9 @@
       <c r="D165" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E165" s="3"/>
+      <c r="E165" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="6" t="s">
@@ -2201,7 +2277,9 @@
       <c r="D166" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E166" s="3"/>
+      <c r="E166" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="6" t="s">
@@ -2216,7 +2294,9 @@
       <c r="D167" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E167" s="3"/>
+      <c r="E167" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="6" t="s">
@@ -2231,7 +2311,9 @@
       <c r="D168" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E168" s="3"/>
+      <c r="E168" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="6" t="s">
@@ -2246,7 +2328,9 @@
       <c r="D169" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E169" s="3"/>
+      <c r="E169" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="6" t="s">
@@ -2261,28 +2345,36 @@
       <c r="D170" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E170" s="3"/>
+      <c r="E170" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="6"/>
       <c r="B171" s="6"/>
       <c r="C171" s="6"/>
       <c r="D171" s="7"/>
-      <c r="E171" s="3"/>
+      <c r="E171" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="6"/>
       <c r="B172" s="6"/>
       <c r="C172" s="6"/>
       <c r="D172" s="7"/>
-      <c r="E172" s="3"/>
+      <c r="E172" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="6"/>
       <c r="B173" s="6"/>
       <c r="C173" s="6"/>
       <c r="D173" s="7"/>
-      <c r="E173" s="3"/>
+      <c r="E173" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="6"/>
@@ -2291,7 +2383,9 @@
         <v>34</v>
       </c>
       <c r="D174" s="7"/>
-      <c r="E174" s="3"/>
+      <c r="E174" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="6"/>
@@ -2300,7 +2394,9 @@
         <v>1</v>
       </c>
       <c r="D175" s="7"/>
-      <c r="E175" s="3"/>
+      <c r="E175" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="6"/>
@@ -2313,7 +2409,9 @@
       <c r="D176" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E176" s="3"/>
+      <c r="E176" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="6"/>
@@ -2322,7 +2420,9 @@
         <v>1</v>
       </c>
       <c r="D177" s="7"/>
-      <c r="E177" s="3"/>
+      <c r="E177" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="6"/>
@@ -2331,7 +2431,9 @@
       </c>
       <c r="C178" s="6"/>
       <c r="D178" s="7"/>
-      <c r="E178" s="3"/>
+      <c r="E178" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="6"/>
@@ -2340,7 +2442,9 @@
       </c>
       <c r="C179" s="6"/>
       <c r="D179" s="7"/>
-      <c r="E179" s="3"/>
+      <c r="E179" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="6" t="s">
@@ -2355,7 +2459,9 @@
       <c r="D180" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E180" s="3"/>
+      <c r="E180" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="6"/>
@@ -2364,14 +2470,18 @@
       </c>
       <c r="C181" s="6"/>
       <c r="D181" s="7"/>
-      <c r="E181" s="3"/>
+      <c r="E181" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="6"/>
       <c r="B182" s="6"/>
       <c r="C182" s="6"/>
       <c r="D182" s="7"/>
-      <c r="E182" s="3"/>
+      <c r="E182" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="6"/>
@@ -2380,7 +2490,9 @@
         <v>1</v>
       </c>
       <c r="D183" s="7"/>
-      <c r="E183" s="3"/>
+      <c r="E183" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="6" t="s">
@@ -2395,8 +2507,8 @@
       <c r="D184" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E184" s="3" t="s">
-        <v>21</v>
+      <c r="E184" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -2406,7 +2518,9 @@
         <v>1</v>
       </c>
       <c r="D185" s="7"/>
-      <c r="E185" s="3"/>
+      <c r="E185" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="6"/>
@@ -2415,35 +2529,45 @@
         <v>34</v>
       </c>
       <c r="D186" s="7"/>
-      <c r="E186" s="3"/>
+      <c r="E186" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="6"/>
       <c r="B187" s="6"/>
       <c r="C187" s="6"/>
       <c r="D187" s="7"/>
-      <c r="E187" s="3"/>
+      <c r="E187" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="6"/>
       <c r="B188" s="6"/>
       <c r="C188" s="6"/>
       <c r="D188" s="7"/>
-      <c r="E188" s="3"/>
+      <c r="E188" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="6"/>
       <c r="B189" s="6"/>
       <c r="C189" s="6"/>
       <c r="D189" s="7"/>
-      <c r="E189" s="3"/>
+      <c r="E189" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="6"/>
       <c r="B190" s="6"/>
       <c r="C190" s="6"/>
       <c r="D190" s="7"/>
-      <c r="E190" s="3"/>
+      <c r="E190" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="6" t="s">
@@ -2458,21 +2582,27 @@
       <c r="D191" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E191" s="3"/>
+      <c r="E191" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="6"/>
       <c r="B192" s="6"/>
       <c r="C192" s="6"/>
       <c r="D192" s="7"/>
-      <c r="E192" s="3"/>
+      <c r="E192" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="6"/>
       <c r="B193" s="6"/>
       <c r="C193" s="6"/>
       <c r="D193" s="7"/>
-      <c r="E193" s="3"/>
+      <c r="E193" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="6"/>
@@ -2483,7 +2613,9 @@
       <c r="D194" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E194" s="3"/>
+      <c r="E194" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="6"/>
@@ -2494,7 +2626,9 @@
       <c r="D195" s="7">
         <v>1</v>
       </c>
-      <c r="E195" s="3"/>
+      <c r="E195" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="6"/>
@@ -2505,7 +2639,9 @@
       <c r="D196" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E196" s="3"/>
+      <c r="E196" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="6" t="s">
@@ -2520,7 +2656,9 @@
       <c r="D197" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E197" s="3"/>
+      <c r="E197" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="6" t="s">
@@ -2535,7 +2673,9 @@
       <c r="D198" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E198" s="3"/>
+      <c r="E198" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="6" t="s">
@@ -2546,7 +2686,9 @@
         <v>34</v>
       </c>
       <c r="D199" s="7"/>
-      <c r="E199" s="3"/>
+      <c r="E199" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="6">
@@ -2557,7 +2699,9 @@
         <v>1</v>
       </c>
       <c r="D200" s="7"/>
-      <c r="E200" s="3"/>
+      <c r="E200" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="6" t="s">
@@ -2568,84 +2712,108 @@
         <v>34</v>
       </c>
       <c r="D201" s="7"/>
-      <c r="E201" s="3"/>
+      <c r="E201" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="6"/>
       <c r="B202" s="6"/>
       <c r="C202" s="6"/>
       <c r="D202" s="7"/>
-      <c r="E202" s="3"/>
+      <c r="E202" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="6"/>
       <c r="B203" s="6"/>
       <c r="C203" s="6"/>
       <c r="D203" s="7"/>
-      <c r="E203" s="3"/>
+      <c r="E203" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="6"/>
       <c r="B204" s="6"/>
       <c r="C204" s="6"/>
       <c r="D204" s="7"/>
-      <c r="E204" s="3"/>
+      <c r="E204" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="6"/>
       <c r="B205" s="6"/>
       <c r="C205" s="6"/>
       <c r="D205" s="7"/>
-      <c r="E205" s="3"/>
+      <c r="E205" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="6"/>
       <c r="B206" s="6"/>
       <c r="C206" s="6"/>
       <c r="D206" s="7"/>
-      <c r="E206" s="3"/>
+      <c r="E206" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="6"/>
       <c r="B207" s="6"/>
       <c r="C207" s="6"/>
       <c r="D207" s="7"/>
-      <c r="E207" s="3"/>
+      <c r="E207" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="6"/>
       <c r="B208" s="6"/>
       <c r="C208" s="6"/>
       <c r="D208" s="7"/>
-      <c r="E208" s="3"/>
+      <c r="E208" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="6"/>
       <c r="B209" s="6"/>
       <c r="C209" s="6"/>
       <c r="D209" s="7"/>
-      <c r="E209" s="3"/>
+      <c r="E209" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="6"/>
       <c r="B210" s="6"/>
       <c r="C210" s="6"/>
       <c r="D210" s="7"/>
-      <c r="E210" s="3"/>
+      <c r="E210" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="6"/>
       <c r="B211" s="6"/>
       <c r="C211" s="6"/>
       <c r="D211" s="7"/>
-      <c r="E211" s="3"/>
+      <c r="E211" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="6"/>
       <c r="B212" s="6"/>
       <c r="C212" s="6"/>
       <c r="D212" s="7"/>
-      <c r="E212" s="3"/>
+      <c r="E212" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="6"/>
@@ -2656,7 +2824,9 @@
         <v>11</v>
       </c>
       <c r="D213" s="7"/>
-      <c r="E213" s="3"/>
+      <c r="E213" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="6"/>
@@ -2667,7 +2837,9 @@
         <v>11</v>
       </c>
       <c r="D214" s="7"/>
-      <c r="E214" s="3"/>
+      <c r="E214" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="6" t="s">
@@ -2682,7 +2854,9 @@
       <c r="D215" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E215" s="3"/>
+      <c r="E215" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="6"/>
@@ -2693,7 +2867,9 @@
         <v>11</v>
       </c>
       <c r="D216" s="7"/>
-      <c r="E216" s="3"/>
+      <c r="E216" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="6"/>
@@ -2704,35 +2880,45 @@
         <v>11</v>
       </c>
       <c r="D217" s="7"/>
-      <c r="E217" s="3"/>
+      <c r="E217" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="6"/>
       <c r="B218" s="6"/>
       <c r="C218" s="6"/>
       <c r="D218" s="7"/>
-      <c r="E218" s="3"/>
+      <c r="E218" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="6"/>
       <c r="B219" s="6"/>
       <c r="C219" s="6"/>
       <c r="D219" s="7"/>
-      <c r="E219" s="3"/>
+      <c r="E219" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="6"/>
       <c r="B220" s="6"/>
       <c r="C220" s="6"/>
       <c r="D220" s="7"/>
-      <c r="E220" s="3"/>
+      <c r="E220" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="6"/>
       <c r="B221" s="6"/>
       <c r="C221" s="6"/>
       <c r="D221" s="7"/>
-      <c r="E221" s="3"/>
+      <c r="E221" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="6" t="s">
@@ -2747,21 +2933,27 @@
       <c r="D222" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E222" s="3"/>
+      <c r="E222" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="6"/>
       <c r="B223" s="6"/>
       <c r="C223" s="6"/>
       <c r="D223" s="7"/>
-      <c r="E223" s="3"/>
+      <c r="E223" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="6"/>
       <c r="B224" s="6"/>
       <c r="C224" s="6"/>
       <c r="D224" s="7"/>
-      <c r="E224" s="3"/>
+      <c r="E224" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="6"/>
@@ -2772,7 +2964,9 @@
         <v>11</v>
       </c>
       <c r="D225" s="7"/>
-      <c r="E225" s="3"/>
+      <c r="E225" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="6"/>
@@ -2783,7 +2977,9 @@
         <v>11</v>
       </c>
       <c r="D226" s="7"/>
-      <c r="E226" s="3"/>
+      <c r="E226" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="6"/>
@@ -2794,7 +2990,9 @@
         <v>11</v>
       </c>
       <c r="D227" s="7"/>
-      <c r="E227" s="3"/>
+      <c r="E227" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="6"/>
@@ -2805,21 +3003,27 @@
         <v>11</v>
       </c>
       <c r="D228" s="7"/>
-      <c r="E228" s="3"/>
+      <c r="E228" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="6"/>
       <c r="B229" s="6"/>
       <c r="C229" s="6"/>
       <c r="D229" s="7"/>
-      <c r="E229" s="3"/>
+      <c r="E229" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="6"/>
       <c r="B230" s="6"/>
       <c r="C230" s="6"/>
       <c r="D230" s="7"/>
-      <c r="E230" s="3"/>
+      <c r="E230" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="6"/>
@@ -2830,7 +3034,9 @@
         <v>14</v>
       </c>
       <c r="D231" s="7"/>
-      <c r="E231" s="3"/>
+      <c r="E231" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="6"/>
@@ -2841,7 +3047,9 @@
         <v>14</v>
       </c>
       <c r="D232" s="7"/>
-      <c r="E232" s="3"/>
+      <c r="E232" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="6"/>
@@ -2852,7 +3060,9 @@
         <v>14</v>
       </c>
       <c r="D233" s="7"/>
-      <c r="E233" s="3"/>
+      <c r="E233" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="6"/>
@@ -2863,7 +3073,9 @@
         <v>14</v>
       </c>
       <c r="D234" s="7"/>
-      <c r="E234" s="3"/>
+      <c r="E234" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="6" t="s">
@@ -2878,7 +3090,9 @@
       <c r="D235" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E235" s="3"/>
+      <c r="E235" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="6" t="s">
@@ -2893,7 +3107,9 @@
       <c r="D236" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E236" s="3"/>
+      <c r="E236" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="6"/>
@@ -2904,7 +3120,9 @@
         <v>14</v>
       </c>
       <c r="D237" s="7"/>
-      <c r="E237" s="3"/>
+      <c r="E237" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="6"/>
@@ -2915,7 +3133,9 @@
         <v>14</v>
       </c>
       <c r="D238" s="7"/>
-      <c r="E238" s="3"/>
+      <c r="E238" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="6"/>
@@ -2926,7 +3146,9 @@
         <v>14</v>
       </c>
       <c r="D239" s="7"/>
-      <c r="E239" s="3"/>
+      <c r="E239" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="6"/>
@@ -2937,7 +3159,9 @@
         <v>14</v>
       </c>
       <c r="D240" s="7"/>
-      <c r="E240" s="3"/>
+      <c r="E240" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="6"/>
@@ -2948,7 +3172,9 @@
         <v>14</v>
       </c>
       <c r="D241" s="7"/>
-      <c r="E241" s="3"/>
+      <c r="E241" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="6"/>
@@ -2959,7 +3185,9 @@
         <v>14</v>
       </c>
       <c r="D242" s="7"/>
-      <c r="E242" s="3"/>
+      <c r="E242" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="6"/>

</xml_diff>

<commit_message>
Added line offset deviation
</commit_message>
<xml_diff>
--- a/Assets/Sources/Tracks/level_1.xlsx
+++ b/Assets/Sources/Tracks/level_1.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="480" yWindow="75" windowWidth="37395" windowHeight="17310"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="level_1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="68">
   <si>
     <t>M</t>
   </si>
@@ -142,6 +142,84 @@
   </si>
   <si>
     <t>shift right</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>shift up</t>
+  </si>
+  <si>
+    <t>shift down</t>
+  </si>
+  <si>
+    <t>ll</t>
+  </si>
+  <si>
+    <t>rr</t>
+  </si>
+  <si>
+    <t>uu</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>uuu</t>
+  </si>
+  <si>
+    <t>ddd</t>
+  </si>
+  <si>
+    <t>lu</t>
+  </si>
+  <si>
+    <t>ru</t>
+  </si>
+  <si>
+    <t>rd</t>
+  </si>
+  <si>
+    <t>ld</t>
+  </si>
+  <si>
+    <t>drr</t>
+  </si>
+  <si>
+    <t>ull</t>
+  </si>
+  <si>
+    <t>dddr</t>
+  </si>
+  <si>
+    <t>drrr</t>
+  </si>
+  <si>
+    <t>uuul</t>
+  </si>
+  <si>
+    <t>ulll</t>
+  </si>
+  <si>
+    <t>dddl</t>
+  </si>
+  <si>
+    <t>dll</t>
+  </si>
+  <si>
+    <t>dlll</t>
+  </si>
+  <si>
+    <t>urrr</t>
+  </si>
+  <si>
+    <t>urr</t>
+  </si>
+  <si>
+    <t>uuur</t>
   </si>
 </sst>
 </file>
@@ -239,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -266,6 +344,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -569,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q478"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A322" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B358" sqref="B358:C360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,8 +803,12 @@
       <c r="L6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
+      <c r="M6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
@@ -754,8 +837,12 @@
       <c r="L7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
+      <c r="M7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -1051,9 +1138,7 @@
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
-      <c r="C38" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="C38" s="6"/>
       <c r="D38" s="7"/>
       <c r="E38" s="3"/>
     </row>
@@ -1952,31 +2037,47 @@
       <c r="E132" s="3"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" s="6"/>
+      <c r="A133" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="B133" s="6"/>
       <c r="C133" s="6"/>
-      <c r="D133" s="7"/>
+      <c r="D133" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="E133" s="3"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" s="6"/>
+      <c r="A134" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="B134" s="6"/>
       <c r="C134" s="6"/>
-      <c r="D134" s="7"/>
+      <c r="D134" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="E134" s="3"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" s="6"/>
+      <c r="A135" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="B135" s="6"/>
       <c r="C135" s="6"/>
-      <c r="D135" s="7"/>
+      <c r="D135" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="E135" s="3"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" s="6"/>
+      <c r="A136" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="B136" s="6"/>
       <c r="C136" s="6"/>
-      <c r="D136" s="7"/>
+      <c r="D136" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="E136" s="3"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -1988,7 +2089,7 @@
         <v>14</v>
       </c>
       <c r="D137" s="7"/>
-      <c r="E137" t="s">
+      <c r="E137" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1997,7 +2098,7 @@
       <c r="B138" s="6"/>
       <c r="C138" s="6"/>
       <c r="D138" s="7"/>
-      <c r="E138" t="s">
+      <c r="E138" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2006,7 +2107,7 @@
       <c r="B139" s="6"/>
       <c r="C139" s="6"/>
       <c r="D139" s="7"/>
-      <c r="E139" t="s">
+      <c r="E139" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2015,7 +2116,7 @@
       <c r="B140" s="6"/>
       <c r="C140" s="6"/>
       <c r="D140" s="7"/>
-      <c r="E140" t="s">
+      <c r="E140" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2024,7 +2125,7 @@
       <c r="B141" s="6"/>
       <c r="C141" s="6"/>
       <c r="D141" s="7"/>
-      <c r="E141" t="s">
+      <c r="E141" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2033,7 +2134,7 @@
       <c r="B142" s="6"/>
       <c r="C142" s="6"/>
       <c r="D142" s="7"/>
-      <c r="E142" t="s">
+      <c r="E142" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2042,7 +2143,7 @@
       <c r="B143" s="6"/>
       <c r="C143" s="6"/>
       <c r="D143" s="7"/>
-      <c r="E143" t="s">
+      <c r="E143" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2051,7 +2152,7 @@
       <c r="B144" s="6"/>
       <c r="C144" s="6"/>
       <c r="D144" s="7"/>
-      <c r="E144" t="s">
+      <c r="E144" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2060,7 +2161,7 @@
       <c r="B145" s="6"/>
       <c r="C145" s="6"/>
       <c r="D145" s="7"/>
-      <c r="E145" t="s">
+      <c r="E145" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2069,7 +2170,7 @@
       <c r="B146" s="6"/>
       <c r="C146" s="6"/>
       <c r="D146" s="7"/>
-      <c r="E146" t="s">
+      <c r="E146" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2078,7 +2179,7 @@
       <c r="B147" s="6"/>
       <c r="C147" s="6"/>
       <c r="D147" s="7"/>
-      <c r="E147" t="s">
+      <c r="E147" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2087,7 +2188,7 @@
       <c r="B148" s="6"/>
       <c r="C148" s="6"/>
       <c r="D148" s="7"/>
-      <c r="E148" t="s">
+      <c r="E148" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2096,7 +2197,7 @@
       <c r="B149" s="6"/>
       <c r="C149" s="6"/>
       <c r="D149" s="7"/>
-      <c r="E149" t="s">
+      <c r="E149" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2105,7 +2206,7 @@
       <c r="B150" s="6"/>
       <c r="C150" s="6"/>
       <c r="D150" s="7"/>
-      <c r="E150" t="s">
+      <c r="E150" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2114,7 +2215,7 @@
       <c r="B151" s="6"/>
       <c r="C151" s="6"/>
       <c r="D151" s="7"/>
-      <c r="E151" t="s">
+      <c r="E151" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2127,7 +2228,7 @@
         <v>6</v>
       </c>
       <c r="D152" s="7"/>
-      <c r="E152" t="s">
+      <c r="E152" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2136,7 +2237,7 @@
       <c r="B153" s="6"/>
       <c r="C153" s="6"/>
       <c r="D153" s="7"/>
-      <c r="E153" t="s">
+      <c r="E153" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2145,7 +2246,7 @@
       <c r="B154" s="6"/>
       <c r="C154" s="6"/>
       <c r="D154" s="7"/>
-      <c r="E154" t="s">
+      <c r="E154" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2154,7 +2255,7 @@
       <c r="B155" s="6"/>
       <c r="C155" s="6"/>
       <c r="D155" s="7"/>
-      <c r="E155" t="s">
+      <c r="E155" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2163,7 +2264,7 @@
       <c r="B156" s="6"/>
       <c r="C156" s="6"/>
       <c r="D156" s="7"/>
-      <c r="E156" t="s">
+      <c r="E156" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2172,7 +2273,7 @@
       <c r="B157" s="6"/>
       <c r="C157" s="6"/>
       <c r="D157" s="7"/>
-      <c r="E157" t="s">
+      <c r="E157" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2181,7 +2282,7 @@
       <c r="B158" s="6"/>
       <c r="C158" s="6"/>
       <c r="D158" s="7"/>
-      <c r="E158" t="s">
+      <c r="E158" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2190,7 +2291,7 @@
       <c r="B159" s="6"/>
       <c r="C159" s="6"/>
       <c r="D159" s="7"/>
-      <c r="E159" t="s">
+      <c r="E159" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2199,7 +2300,7 @@
       <c r="B160" s="6"/>
       <c r="C160" s="6"/>
       <c r="D160" s="7"/>
-      <c r="E160" t="s">
+      <c r="E160" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2208,7 +2309,7 @@
       <c r="B161" s="6"/>
       <c r="C161" s="6"/>
       <c r="D161" s="7"/>
-      <c r="E161" t="s">
+      <c r="E161" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2217,7 +2318,7 @@
       <c r="B162" s="6"/>
       <c r="C162" s="6"/>
       <c r="D162" s="7"/>
-      <c r="E162" t="s">
+      <c r="E162" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2226,7 +2327,7 @@
       <c r="B163" s="6"/>
       <c r="C163" s="6"/>
       <c r="D163" s="7"/>
-      <c r="E163" t="s">
+      <c r="E163" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2243,7 +2344,7 @@
       <c r="D164" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E164" t="s">
+      <c r="E164" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2260,7 +2361,7 @@
       <c r="D165" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2277,7 +2378,7 @@
       <c r="D166" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2294,7 +2395,7 @@
       <c r="D167" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2311,7 +2412,7 @@
       <c r="D168" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E168" t="s">
+      <c r="E168" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2328,7 +2429,7 @@
       <c r="D169" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2345,7 +2446,7 @@
       <c r="D170" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2354,7 +2455,7 @@
       <c r="B171" s="6"/>
       <c r="C171" s="6"/>
       <c r="D171" s="7"/>
-      <c r="E171" t="s">
+      <c r="E171" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2363,7 +2464,7 @@
       <c r="B172" s="6"/>
       <c r="C172" s="6"/>
       <c r="D172" s="7"/>
-      <c r="E172" t="s">
+      <c r="E172" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2372,7 +2473,7 @@
       <c r="B173" s="6"/>
       <c r="C173" s="6"/>
       <c r="D173" s="7"/>
-      <c r="E173" t="s">
+      <c r="E173" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2383,7 +2484,7 @@
         <v>34</v>
       </c>
       <c r="D174" s="7"/>
-      <c r="E174" t="s">
+      <c r="E174" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2394,7 +2495,7 @@
         <v>1</v>
       </c>
       <c r="D175" s="7"/>
-      <c r="E175" t="s">
+      <c r="E175" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2409,7 +2510,7 @@
       <c r="D176" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E176" t="s">
+      <c r="E176" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2420,7 +2521,7 @@
         <v>1</v>
       </c>
       <c r="D177" s="7"/>
-      <c r="E177" t="s">
+      <c r="E177" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2431,7 +2532,7 @@
       </c>
       <c r="C178" s="6"/>
       <c r="D178" s="7"/>
-      <c r="E178" t="s">
+      <c r="E178" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2442,7 +2543,7 @@
       </c>
       <c r="C179" s="6"/>
       <c r="D179" s="7"/>
-      <c r="E179" t="s">
+      <c r="E179" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2459,7 +2560,7 @@
       <c r="D180" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E180" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2470,7 +2571,7 @@
       </c>
       <c r="C181" s="6"/>
       <c r="D181" s="7"/>
-      <c r="E181" t="s">
+      <c r="E181" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2479,7 +2580,7 @@
       <c r="B182" s="6"/>
       <c r="C182" s="6"/>
       <c r="D182" s="7"/>
-      <c r="E182" t="s">
+      <c r="E182" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2490,7 +2591,7 @@
         <v>1</v>
       </c>
       <c r="D183" s="7"/>
-      <c r="E183" t="s">
+      <c r="E183" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2507,7 +2608,7 @@
       <c r="D184" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E184" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2518,7 +2619,7 @@
         <v>1</v>
       </c>
       <c r="D185" s="7"/>
-      <c r="E185" t="s">
+      <c r="E185" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2529,7 +2630,7 @@
         <v>34</v>
       </c>
       <c r="D186" s="7"/>
-      <c r="E186" t="s">
+      <c r="E186" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2538,7 +2639,7 @@
       <c r="B187" s="6"/>
       <c r="C187" s="6"/>
       <c r="D187" s="7"/>
-      <c r="E187" t="s">
+      <c r="E187" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2547,7 +2648,7 @@
       <c r="B188" s="6"/>
       <c r="C188" s="6"/>
       <c r="D188" s="7"/>
-      <c r="E188" t="s">
+      <c r="E188" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2556,7 +2657,7 @@
       <c r="B189" s="6"/>
       <c r="C189" s="6"/>
       <c r="D189" s="7"/>
-      <c r="E189" t="s">
+      <c r="E189" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2565,7 +2666,7 @@
       <c r="B190" s="6"/>
       <c r="C190" s="6"/>
       <c r="D190" s="7"/>
-      <c r="E190" t="s">
+      <c r="E190" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2582,7 +2683,7 @@
       <c r="D191" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E191" t="s">
+      <c r="E191" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2591,7 +2692,7 @@
       <c r="B192" s="6"/>
       <c r="C192" s="6"/>
       <c r="D192" s="7"/>
-      <c r="E192" t="s">
+      <c r="E192" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2600,7 +2701,7 @@
       <c r="B193" s="6"/>
       <c r="C193" s="6"/>
       <c r="D193" s="7"/>
-      <c r="E193" t="s">
+      <c r="E193" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2613,7 +2714,7 @@
       <c r="D194" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E194" t="s">
+      <c r="E194" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2626,7 +2727,7 @@
       <c r="D195" s="7">
         <v>1</v>
       </c>
-      <c r="E195" t="s">
+      <c r="E195" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2639,7 +2740,7 @@
       <c r="D196" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E196" t="s">
+      <c r="E196" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2656,7 +2757,7 @@
       <c r="D197" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E197" t="s">
+      <c r="E197" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2673,7 +2774,7 @@
       <c r="D198" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E198" t="s">
+      <c r="E198" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2686,7 +2787,7 @@
         <v>34</v>
       </c>
       <c r="D199" s="7"/>
-      <c r="E199" t="s">
+      <c r="E199" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2699,7 +2800,7 @@
         <v>1</v>
       </c>
       <c r="D200" s="7"/>
-      <c r="E200" t="s">
+      <c r="E200" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2712,7 +2813,7 @@
         <v>34</v>
       </c>
       <c r="D201" s="7"/>
-      <c r="E201" t="s">
+      <c r="E201" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2721,7 +2822,7 @@
       <c r="B202" s="6"/>
       <c r="C202" s="6"/>
       <c r="D202" s="7"/>
-      <c r="E202" t="s">
+      <c r="E202" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2730,7 +2831,7 @@
       <c r="B203" s="6"/>
       <c r="C203" s="6"/>
       <c r="D203" s="7"/>
-      <c r="E203" t="s">
+      <c r="E203" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2739,7 +2840,7 @@
       <c r="B204" s="6"/>
       <c r="C204" s="6"/>
       <c r="D204" s="7"/>
-      <c r="E204" t="s">
+      <c r="E204" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2748,7 +2849,7 @@
       <c r="B205" s="6"/>
       <c r="C205" s="6"/>
       <c r="D205" s="7"/>
-      <c r="E205" t="s">
+      <c r="E205" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2757,7 +2858,7 @@
       <c r="B206" s="6"/>
       <c r="C206" s="6"/>
       <c r="D206" s="7"/>
-      <c r="E206" t="s">
+      <c r="E206" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2766,7 +2867,7 @@
       <c r="B207" s="6"/>
       <c r="C207" s="6"/>
       <c r="D207" s="7"/>
-      <c r="E207" t="s">
+      <c r="E207" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2775,7 +2876,7 @@
       <c r="B208" s="6"/>
       <c r="C208" s="6"/>
       <c r="D208" s="7"/>
-      <c r="E208" t="s">
+      <c r="E208" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2784,7 +2885,7 @@
       <c r="B209" s="6"/>
       <c r="C209" s="6"/>
       <c r="D209" s="7"/>
-      <c r="E209" t="s">
+      <c r="E209" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2793,7 +2894,7 @@
       <c r="B210" s="6"/>
       <c r="C210" s="6"/>
       <c r="D210" s="7"/>
-      <c r="E210" t="s">
+      <c r="E210" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2802,7 +2903,7 @@
       <c r="B211" s="6"/>
       <c r="C211" s="6"/>
       <c r="D211" s="7"/>
-      <c r="E211" t="s">
+      <c r="E211" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2811,7 +2912,7 @@
       <c r="B212" s="6"/>
       <c r="C212" s="6"/>
       <c r="D212" s="7"/>
-      <c r="E212" t="s">
+      <c r="E212" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2824,7 +2925,7 @@
         <v>11</v>
       </c>
       <c r="D213" s="7"/>
-      <c r="E213" t="s">
+      <c r="E213" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2837,7 +2938,7 @@
         <v>11</v>
       </c>
       <c r="D214" s="7"/>
-      <c r="E214" t="s">
+      <c r="E214" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2854,7 +2955,7 @@
       <c r="D215" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E215" t="s">
+      <c r="E215" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2867,7 +2968,7 @@
         <v>11</v>
       </c>
       <c r="D216" s="7"/>
-      <c r="E216" t="s">
+      <c r="E216" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2880,7 +2981,7 @@
         <v>11</v>
       </c>
       <c r="D217" s="7"/>
-      <c r="E217" t="s">
+      <c r="E217" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2889,7 +2990,7 @@
       <c r="B218" s="6"/>
       <c r="C218" s="6"/>
       <c r="D218" s="7"/>
-      <c r="E218" t="s">
+      <c r="E218" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2898,7 +2999,7 @@
       <c r="B219" s="6"/>
       <c r="C219" s="6"/>
       <c r="D219" s="7"/>
-      <c r="E219" t="s">
+      <c r="E219" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2907,7 +3008,7 @@
       <c r="B220" s="6"/>
       <c r="C220" s="6"/>
       <c r="D220" s="7"/>
-      <c r="E220" t="s">
+      <c r="E220" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2916,7 +3017,7 @@
       <c r="B221" s="6"/>
       <c r="C221" s="6"/>
       <c r="D221" s="7"/>
-      <c r="E221" t="s">
+      <c r="E221" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2933,7 +3034,7 @@
       <c r="D222" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E222" t="s">
+      <c r="E222" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2942,7 +3043,7 @@
       <c r="B223" s="6"/>
       <c r="C223" s="6"/>
       <c r="D223" s="7"/>
-      <c r="E223" t="s">
+      <c r="E223" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2951,7 +3052,7 @@
       <c r="B224" s="6"/>
       <c r="C224" s="6"/>
       <c r="D224" s="7"/>
-      <c r="E224" t="s">
+      <c r="E224" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2964,7 +3065,7 @@
         <v>11</v>
       </c>
       <c r="D225" s="7"/>
-      <c r="E225" t="s">
+      <c r="E225" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2977,7 +3078,7 @@
         <v>11</v>
       </c>
       <c r="D226" s="7"/>
-      <c r="E226" t="s">
+      <c r="E226" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2990,7 +3091,7 @@
         <v>11</v>
       </c>
       <c r="D227" s="7"/>
-      <c r="E227" t="s">
+      <c r="E227" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3003,7 +3104,7 @@
         <v>11</v>
       </c>
       <c r="D228" s="7"/>
-      <c r="E228" t="s">
+      <c r="E228" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3012,7 +3113,7 @@
       <c r="B229" s="6"/>
       <c r="C229" s="6"/>
       <c r="D229" s="7"/>
-      <c r="E229" t="s">
+      <c r="E229" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3021,7 +3122,7 @@
       <c r="B230" s="6"/>
       <c r="C230" s="6"/>
       <c r="D230" s="7"/>
-      <c r="E230" t="s">
+      <c r="E230" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3034,7 +3135,7 @@
         <v>14</v>
       </c>
       <c r="D231" s="7"/>
-      <c r="E231" t="s">
+      <c r="E231" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3047,7 +3148,7 @@
         <v>14</v>
       </c>
       <c r="D232" s="7"/>
-      <c r="E232" t="s">
+      <c r="E232" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3060,7 +3161,7 @@
         <v>14</v>
       </c>
       <c r="D233" s="7"/>
-      <c r="E233" t="s">
+      <c r="E233" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3073,7 +3174,7 @@
         <v>14</v>
       </c>
       <c r="D234" s="7"/>
-      <c r="E234" t="s">
+      <c r="E234" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3090,7 +3191,7 @@
       <c r="D235" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E235" t="s">
+      <c r="E235" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3107,7 +3208,7 @@
       <c r="D236" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E236" t="s">
+      <c r="E236" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3120,7 +3221,7 @@
         <v>14</v>
       </c>
       <c r="D237" s="7"/>
-      <c r="E237" t="s">
+      <c r="E237" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3133,7 +3234,7 @@
         <v>14</v>
       </c>
       <c r="D238" s="7"/>
-      <c r="E238" t="s">
+      <c r="E238" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3146,7 +3247,7 @@
         <v>14</v>
       </c>
       <c r="D239" s="7"/>
-      <c r="E239" t="s">
+      <c r="E239" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3159,7 +3260,7 @@
         <v>14</v>
       </c>
       <c r="D240" s="7"/>
-      <c r="E240" t="s">
+      <c r="E240" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3172,7 +3273,7 @@
         <v>14</v>
       </c>
       <c r="D241" s="7"/>
-      <c r="E241" t="s">
+      <c r="E241" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3185,7 +3286,7 @@
         <v>14</v>
       </c>
       <c r="D242" s="7"/>
-      <c r="E242" t="s">
+      <c r="E242" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3212,47 +3313,63 @@
       <c r="E244" s="3"/>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A245" s="6"/>
+      <c r="A245" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="B245" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C245" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D245" s="7"/>
+      <c r="D245" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="E245" s="3"/>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A246" s="6"/>
+      <c r="A246" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="B246" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C246" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D246" s="7"/>
+      <c r="D246" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="E246" s="3"/>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A247" s="6"/>
+      <c r="A247" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="B247" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C247" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D247" s="7"/>
+      <c r="D247" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="E247" s="3"/>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A248" s="6"/>
+      <c r="A248" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="B248" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C248" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D248" s="7"/>
+      <c r="D248" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="E248" s="3"/>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
@@ -3691,52 +3808,80 @@
       <c r="E293" s="3"/>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A294" s="6"/>
+      <c r="A294" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="B294" s="6"/>
       <c r="C294" s="6"/>
-      <c r="D294" s="7"/>
+      <c r="D294" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="E294" s="3"/>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A295" s="6"/>
+      <c r="A295" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="B295" s="6"/>
       <c r="C295" s="6"/>
-      <c r="D295" s="7"/>
+      <c r="D295" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="E295" s="3"/>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A296" s="6"/>
+      <c r="A296" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="B296" s="6"/>
       <c r="C296" s="6"/>
-      <c r="D296" s="7"/>
+      <c r="D296" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="E296" s="3"/>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A297" s="6"/>
+      <c r="A297" s="6" t="s">
+        <v>62</v>
+      </c>
       <c r="B297" s="6"/>
       <c r="C297" s="6"/>
-      <c r="D297" s="7"/>
+      <c r="D297" s="6" t="s">
+        <v>58</v>
+      </c>
       <c r="E297" s="3"/>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A298" s="6"/>
+      <c r="A298" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B298" s="6"/>
       <c r="C298" s="6"/>
-      <c r="D298" s="7"/>
+      <c r="D298" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="E298" s="3"/>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A299" s="6"/>
+      <c r="A299" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="B299" s="6"/>
       <c r="C299" s="6"/>
-      <c r="D299" s="7"/>
+      <c r="D299" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="E299" s="3"/>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A300" s="6"/>
+      <c r="A300" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="B300" s="6"/>
       <c r="C300" s="6"/>
-      <c r="D300" s="7"/>
+      <c r="D300" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="E300" s="3"/>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
@@ -3920,8 +4065,12 @@
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" s="6"/>
-      <c r="B322" s="6"/>
-      <c r="C322" s="6"/>
+      <c r="B322" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C322" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="D322" s="7"/>
       <c r="E322" s="3" t="s">
         <v>19</v>
@@ -3929,8 +4078,12 @@
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="6"/>
-      <c r="B323" s="6"/>
-      <c r="C323" s="6"/>
+      <c r="B323" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C323" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="D323" s="7"/>
       <c r="E323" s="3" t="s">
         <v>19</v>
@@ -3938,8 +4091,12 @@
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="6"/>
-      <c r="B324" s="6"/>
-      <c r="C324" s="6"/>
+      <c r="B324" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C324" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="D324" s="7"/>
       <c r="E324" s="3" t="s">
         <v>19</v>
@@ -3980,8 +4137,12 @@
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="6"/>
-      <c r="B328" s="6"/>
-      <c r="C328" s="6"/>
+      <c r="B328" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C328" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="D328" s="7"/>
       <c r="E328" s="3" t="s">
         <v>19</v>
@@ -3989,8 +4150,12 @@
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="6"/>
-      <c r="B329" s="6"/>
-      <c r="C329" s="6"/>
+      <c r="B329" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C329" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="D329" s="7"/>
       <c r="E329" s="3" t="s">
         <v>19</v>
@@ -3998,8 +4163,12 @@
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="6"/>
-      <c r="B330" s="6"/>
-      <c r="C330" s="6"/>
+      <c r="B330" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C330" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="D330" s="7"/>
       <c r="E330" s="3" t="s">
         <v>19</v>
@@ -4036,8 +4205,12 @@
       <c r="A334" s="6">
         <v>11</v>
       </c>
-      <c r="B334" s="6"/>
-      <c r="C334" s="6"/>
+      <c r="B334" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C334" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="D334" s="7"/>
       <c r="E334" s="3" t="s">
         <v>1</v>
@@ -4047,8 +4220,12 @@
       <c r="A335" s="6">
         <v>11</v>
       </c>
-      <c r="B335" s="6"/>
-      <c r="C335" s="6"/>
+      <c r="B335" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C335" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="D335" s="7"/>
       <c r="E335" s="3" t="s">
         <v>1</v>
@@ -4058,8 +4235,12 @@
       <c r="A336" s="6">
         <v>11</v>
       </c>
-      <c r="B336" s="6"/>
-      <c r="C336" s="6"/>
+      <c r="B336" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C336" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="D336" s="7"/>
       <c r="E336" s="3" t="s">
         <v>1</v>
@@ -4104,8 +4285,12 @@
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="6"/>
-      <c r="B340" s="6"/>
-      <c r="C340" s="6"/>
+      <c r="B340" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C340" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="D340" s="7"/>
       <c r="E340" s="3" t="s">
         <v>1</v>
@@ -4113,8 +4298,12 @@
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="6"/>
-      <c r="B341" s="6"/>
-      <c r="C341" s="6"/>
+      <c r="B341" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C341" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="D341" s="7"/>
       <c r="E341" s="3" t="s">
         <v>19</v>
@@ -4122,8 +4311,12 @@
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="6"/>
-      <c r="B342" s="6"/>
-      <c r="C342" s="6"/>
+      <c r="B342" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C342" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="D342" s="7"/>
       <c r="E342" s="3" t="s">
         <v>19</v>
@@ -4153,8 +4346,12 @@
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="6"/>
-      <c r="B345" s="6"/>
-      <c r="C345" s="6"/>
+      <c r="B345" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C345" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="D345" s="7">
         <v>11</v>
       </c>
@@ -4164,8 +4361,12 @@
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" s="6"/>
-      <c r="B346" s="6"/>
-      <c r="C346" s="6"/>
+      <c r="B346" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C346" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="D346" s="7">
         <v>11</v>
       </c>
@@ -4175,8 +4376,12 @@
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" s="6"/>
-      <c r="B347" s="6"/>
-      <c r="C347" s="6"/>
+      <c r="B347" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C347" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="D347" s="7"/>
       <c r="E347" s="3" t="s">
         <v>19</v>
@@ -4318,8 +4523,12 @@
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="6"/>
-      <c r="B358" s="6"/>
-      <c r="C358" s="6"/>
+      <c r="B358" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C358" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="D358" s="7"/>
       <c r="E358" s="3" t="s">
         <v>19</v>
@@ -4327,8 +4536,12 @@
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" s="6"/>
-      <c r="B359" s="6"/>
-      <c r="C359" s="6"/>
+      <c r="B359" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C359" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="D359" s="7"/>
       <c r="E359" s="3" t="s">
         <v>19</v>
@@ -4336,8 +4549,12 @@
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" s="6"/>
-      <c r="B360" s="6"/>
-      <c r="C360" s="6"/>
+      <c r="B360" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C360" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="D360" s="7"/>
       <c r="E360" s="3" t="s">
         <v>19</v>
@@ -4455,52 +4672,80 @@
       <c r="E375" s="3"/>
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A376" s="6"/>
+      <c r="A376" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="B376" s="6"/>
       <c r="C376" s="6"/>
-      <c r="D376" s="7"/>
+      <c r="D376" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="E376" s="3"/>
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A377" s="6"/>
+      <c r="A377" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="B377" s="6"/>
       <c r="C377" s="6"/>
-      <c r="D377" s="7"/>
+      <c r="D377" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="E377" s="3"/>
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A378" s="6"/>
+      <c r="A378" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="B378" s="6"/>
       <c r="C378" s="6"/>
-      <c r="D378" s="7"/>
+      <c r="D378" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="E378" s="3"/>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A379" s="6"/>
+      <c r="A379" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="B379" s="6"/>
       <c r="C379" s="6"/>
-      <c r="D379" s="7"/>
+      <c r="D379" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="E379" s="3"/>
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A380" s="6"/>
+      <c r="A380" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="B380" s="6"/>
       <c r="C380" s="6"/>
-      <c r="D380" s="7"/>
+      <c r="D380" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="E380" s="3"/>
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A381" s="6"/>
+      <c r="A381" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="B381" s="6"/>
       <c r="C381" s="6"/>
-      <c r="D381" s="7"/>
+      <c r="D381" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="E381" s="3"/>
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A382" s="6"/>
+      <c r="A382" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="B382" s="6"/>
       <c r="C382" s="6"/>
-      <c r="D382" s="7"/>
+      <c r="D382" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="E382" s="3"/>
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added deathloop to generator, fix pause, add pause for level loading
</commit_message>
<xml_diff>
--- a/Assets/Sources/Tracks/level_1.xlsx
+++ b/Assets/Sources/Tracks/level_1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="65">
   <si>
     <t>M</t>
   </si>
@@ -187,6 +187,30 @@
   </si>
   <si>
     <t>Arrr</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>O+R</t>
+  </si>
+  <si>
+    <t>+R</t>
+  </si>
+  <si>
+    <t>XR</t>
+  </si>
+  <si>
+    <t>11R</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>start deathloop</t>
+  </si>
+  <si>
+    <t>end deathloop</t>
   </si>
 </sst>
 </file>
@@ -617,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A376" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D393" sqref="D393:D397"/>
+    <sheetView tabSelected="1" topLeftCell="B220" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E244" sqref="E244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,8 +802,12 @@
       <c r="N6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
+      <c r="O6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -812,8 +840,12 @@
       <c r="N7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
+      <c r="O7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="Q7" s="1"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -2031,7 +2063,9 @@
       <c r="B136" s="6"/>
       <c r="C136" s="6"/>
       <c r="D136" s="7"/>
-      <c r="E136" s="3"/>
+      <c r="E136" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="6"/>
@@ -3252,7 +3286,9 @@
         <v>14</v>
       </c>
       <c r="D243" s="7"/>
-      <c r="E243" s="3"/>
+      <c r="E243" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="6"/>
@@ -4759,142 +4795,242 @@
       <c r="E399" s="3"/>
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A400" s="6"/>
-      <c r="B400" s="6"/>
-      <c r="C400" s="6"/>
-      <c r="D400" s="7"/>
+      <c r="A400" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B400" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C400" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D400" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="E400" s="3"/>
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A401" s="6"/>
-      <c r="B401" s="6"/>
-      <c r="C401" s="6"/>
-      <c r="D401" s="7"/>
+      <c r="A401" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B401" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C401" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D401" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="E401" s="3"/>
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A402" s="6"/>
-      <c r="B402" s="6"/>
-      <c r="C402" s="6"/>
-      <c r="D402" s="7"/>
+      <c r="A402" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B402" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C402" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D402" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="E402" s="3"/>
     </row>
     <row r="403" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A403" s="6"/>
-      <c r="B403" s="6"/>
-      <c r="C403" s="6"/>
-      <c r="D403" s="7"/>
+      <c r="A403" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B403" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C403" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D403" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="E403" s="3"/>
     </row>
     <row r="404" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A404" s="6"/>
-      <c r="B404" s="6"/>
-      <c r="C404" s="6"/>
-      <c r="D404" s="7"/>
+      <c r="A404" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B404" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C404" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D404" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="E404" s="3"/>
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A405" s="6"/>
-      <c r="B405" s="6"/>
-      <c r="C405" s="6"/>
-      <c r="D405" s="7"/>
+      <c r="A405" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B405" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C405" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D405" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="E405" s="3"/>
     </row>
     <row r="406" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A406" s="6"/>
-      <c r="B406" s="6">
-        <v>11</v>
-      </c>
-      <c r="C406" s="6">
-        <v>11</v>
-      </c>
-      <c r="D406" s="7"/>
+      <c r="A406" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B406" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C406" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D406" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="E406" s="3"/>
     </row>
     <row r="407" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A407" s="6"/>
-      <c r="B407" s="6">
-        <v>11</v>
-      </c>
-      <c r="C407" s="6">
-        <v>11</v>
-      </c>
-      <c r="D407" s="7"/>
+      <c r="A407" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B407" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C407" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D407" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="E407" s="3"/>
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A408" s="6"/>
-      <c r="B408" s="6">
-        <v>11</v>
-      </c>
-      <c r="C408" s="6">
-        <v>11</v>
-      </c>
-      <c r="D408" s="7"/>
+      <c r="A408" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B408" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C408" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D408" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="E408" s="3"/>
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A409" s="6"/>
-      <c r="B409" s="6">
-        <v>11</v>
-      </c>
-      <c r="C409" s="6">
-        <v>11</v>
-      </c>
-      <c r="D409" s="7"/>
+      <c r="A409" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B409" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C409" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D409" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="E409" s="3"/>
     </row>
     <row r="410" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A410" s="6"/>
-      <c r="B410" s="6">
-        <v>11</v>
-      </c>
-      <c r="C410" s="6">
-        <v>11</v>
-      </c>
-      <c r="D410" s="7"/>
+      <c r="A410" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B410" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C410" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D410" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="E410" s="3"/>
     </row>
     <row r="411" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A411" s="6"/>
-      <c r="B411" s="6"/>
-      <c r="C411" s="6"/>
-      <c r="D411" s="7"/>
+      <c r="A411" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B411" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C411" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D411" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="E411" s="3"/>
     </row>
     <row r="412" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A412" s="6"/>
-      <c r="B412" s="6"/>
-      <c r="C412" s="6"/>
-      <c r="D412" s="7"/>
+      <c r="A412" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B412" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C412" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D412" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="E412" s="3"/>
     </row>
     <row r="413" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A413" s="6"/>
-      <c r="B413" s="6"/>
-      <c r="C413" s="6"/>
-      <c r="D413" s="7"/>
+      <c r="A413" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B413" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C413" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D413" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="E413" s="3"/>
     </row>
     <row r="414" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A414" s="6"/>
-      <c r="B414" s="6"/>
-      <c r="C414" s="6"/>
-      <c r="D414" s="7"/>
+      <c r="A414" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B414" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C414" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D414" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="E414" s="3"/>
     </row>
     <row r="415" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A415" s="6" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="B415" s="6" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="C415" s="6" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D415" s="7" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E415" s="3"/>
     </row>
@@ -5004,88 +5140,168 @@
       <c r="E422" s="3"/>
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A423" s="6"/>
-      <c r="B423" s="6"/>
-      <c r="C423" s="6"/>
-      <c r="D423" s="7"/>
+      <c r="A423" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B423" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C423" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D423" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="E423" s="3"/>
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A424" s="6"/>
-      <c r="B424" s="6"/>
-      <c r="C424" s="6"/>
-      <c r="D424" s="7"/>
+      <c r="A424" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B424" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C424" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D424" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="E424" s="3"/>
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A425" s="6"/>
-      <c r="B425" s="6"/>
-      <c r="C425" s="6"/>
-      <c r="D425" s="7"/>
+      <c r="A425" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B425" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C425" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D425" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="E425" s="3"/>
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A426" s="6"/>
-      <c r="B426" s="6"/>
-      <c r="C426" s="6"/>
-      <c r="D426" s="7"/>
+      <c r="A426" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B426" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C426" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D426" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="E426" s="3"/>
     </row>
     <row r="427" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A427" s="6"/>
-      <c r="B427" s="6"/>
-      <c r="C427" s="6"/>
-      <c r="D427" s="7"/>
+      <c r="A427" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B427" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C427" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D427" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="E427" s="3"/>
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A428" s="6" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="B428" s="6" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="C428" s="6" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="D428" s="7" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="E428" s="3"/>
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A429" s="6"/>
-      <c r="B429" s="6"/>
-      <c r="C429" s="6"/>
-      <c r="D429" s="7"/>
+      <c r="A429" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B429" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C429" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D429" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="E429" s="3"/>
     </row>
     <row r="430" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A430" s="6"/>
-      <c r="B430" s="6"/>
-      <c r="C430" s="6"/>
-      <c r="D430" s="7"/>
+      <c r="A430" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B430" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C430" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D430" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="E430" s="3"/>
     </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A431" s="6"/>
-      <c r="B431" s="6"/>
-      <c r="C431" s="6"/>
-      <c r="D431" s="7"/>
+      <c r="A431" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B431" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C431" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D431" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="E431" s="3"/>
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A432" s="6"/>
-      <c r="B432" s="6"/>
-      <c r="C432" s="6"/>
-      <c r="D432" s="7"/>
+      <c r="A432" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B432" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C432" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D432" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="E432" s="3"/>
     </row>
     <row r="433" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A433" s="6"/>
-      <c r="B433" s="6"/>
-      <c r="C433" s="6"/>
-      <c r="D433" s="7"/>
+      <c r="A433" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B433" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C433" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D433" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="E433" s="3"/>
     </row>
     <row r="434" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add track rotation & fences
</commit_message>
<xml_diff>
--- a/Assets/Sources/Tracks/level_1.xlsx
+++ b/Assets/Sources/Tracks/level_1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="37395" windowHeight="17310"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="81">
   <si>
     <t>M</t>
   </si>
@@ -129,9 +129,6 @@
     <t>2</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>r</t>
   </si>
   <si>
@@ -211,6 +208,57 @@
   </si>
   <si>
     <t>end deathloop</t>
+  </si>
+  <si>
+    <t>rotate left</t>
+  </si>
+  <si>
+    <t>rotate right</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>fence</t>
+  </si>
+  <si>
+    <t>----</t>
+  </si>
+  <si>
+    <t>-----</t>
+  </si>
+  <si>
+    <t>L------</t>
+  </si>
+  <si>
+    <t>------</t>
+  </si>
+  <si>
+    <t>--F</t>
+  </si>
+  <si>
+    <t>----F</t>
+  </si>
+  <si>
+    <t>L------F</t>
+  </si>
+  <si>
+    <t>------F</t>
+  </si>
+  <si>
+    <t>-----F</t>
+  </si>
+  <si>
+    <t>---F</t>
+  </si>
+  <si>
+    <t>-F</t>
   </si>
 </sst>
 </file>
@@ -244,7 +292,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -304,11 +352,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -335,9 +420,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -639,10 +736,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Лист1"/>
   <dimension ref="A1:Q478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B220" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E244" sqref="E244"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,20 +755,22 @@
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="7"/>
-      <c r="E1" s="3"/>
-      <c r="G1" s="10" t="s">
+      <c r="E1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -696,28 +796,15 @@
       <c r="L2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="2">
-        <v>1</v>
-      </c>
-      <c r="P2" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>3</v>
-      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
@@ -735,21 +822,6 @@
       </c>
       <c r="L3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -758,19 +830,47 @@
       <c r="C4" s="6"/>
       <c r="D4" s="7"/>
       <c r="E4" s="3"/>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2">
+        <v>3</v>
+      </c>
+      <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="3"/>
-      <c r="G5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
+      <c r="E5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="10"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
@@ -778,75 +878,15 @@
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
       <c r="E6" s="3"/>
-      <c r="G6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="3"/>
-      <c r="G7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q7" s="1"/>
+      <c r="E7" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
@@ -860,7 +900,9 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
@@ -868,13 +910,43 @@
       <c r="C10" s="6"/>
       <c r="D10" s="7"/>
       <c r="E10" s="3"/>
+      <c r="G10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="14"/>
+      <c r="L11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
@@ -882,13 +954,36 @@
       <c r="C12" s="6"/>
       <c r="D12" s="7"/>
       <c r="E12" s="3"/>
+      <c r="G12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="14"/>
+      <c r="L12" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K13" s="14"/>
+      <c r="L13" s="18"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
@@ -896,6 +991,21 @@
       <c r="C14" s="6"/>
       <c r="D14" s="7"/>
       <c r="E14" s="3"/>
+      <c r="G14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K14" s="14"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="10"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
@@ -910,7 +1020,24 @@
       <c r="D15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K15" s="14"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="10"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
@@ -918,29 +1045,61 @@
       <c r="C16" s="6"/>
       <c r="D16" s="7"/>
       <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K16" s="14"/>
+      <c r="L16" s="18"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="10"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="7"/>
       <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="7"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>1</v>
       </c>
@@ -955,7 +1114,7 @@
       </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>1</v>
       </c>
@@ -968,9 +1127,11 @@
       <c r="D21" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>1</v>
       </c>
@@ -985,7 +1146,7 @@
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>1</v>
       </c>
@@ -998,9 +1159,11 @@
       <c r="D23" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>1</v>
       </c>
@@ -1015,7 +1178,7 @@
       </c>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>1</v>
       </c>
@@ -1028,53 +1191,61 @@
       <c r="D25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="7"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="7"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="7"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="7"/>
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -1090,7 +1261,9 @@
         <v>34</v>
       </c>
       <c r="D33" s="7"/>
-      <c r="E33" s="3"/>
+      <c r="E33" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
@@ -1112,7 +1285,9 @@
         <v>34</v>
       </c>
       <c r="D35" s="7"/>
-      <c r="E35" s="3"/>
+      <c r="E35" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
@@ -1123,7 +1298,9 @@
         <v>34</v>
       </c>
       <c r="D36" s="7"/>
-      <c r="E36" s="3"/>
+      <c r="E36" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
@@ -1134,28 +1311,36 @@
         <v>1</v>
       </c>
       <c r="D37" s="7"/>
-      <c r="E37" s="3"/>
+      <c r="E37" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="7"/>
-      <c r="E38" s="3"/>
+      <c r="E38" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="7"/>
-      <c r="E39" s="3"/>
+      <c r="E39" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="7"/>
-      <c r="E40" s="3"/>
+      <c r="E40" s="3" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
@@ -1163,7 +1348,7 @@
       <c r="C41" s="6"/>
       <c r="D41" s="7"/>
       <c r="E41" s="3" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1172,7 +1357,7 @@
       <c r="C42" s="6"/>
       <c r="D42" s="7"/>
       <c r="E42" s="3" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1181,7 +1366,7 @@
       <c r="C43" s="6"/>
       <c r="D43" s="7"/>
       <c r="E43" s="3" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1190,7 +1375,7 @@
       <c r="C44" s="6"/>
       <c r="D44" s="7"/>
       <c r="E44" s="3" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1199,7 +1384,7 @@
       <c r="C45" s="6"/>
       <c r="D45" s="7"/>
       <c r="E45" s="3" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1208,7 +1393,7 @@
       <c r="C46" s="6"/>
       <c r="D46" s="7"/>
       <c r="E46" s="3" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1217,7 +1402,7 @@
       <c r="C47" s="6"/>
       <c r="D47" s="7"/>
       <c r="E47" s="3" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1226,7 +1411,7 @@
       <c r="C48" s="6"/>
       <c r="D48" s="7"/>
       <c r="E48" s="3" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1235,7 +1420,7 @@
       <c r="C49" s="6"/>
       <c r="D49" s="7"/>
       <c r="E49" s="3" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1244,7 +1429,7 @@
       <c r="C50" s="6"/>
       <c r="D50" s="7"/>
       <c r="E50" s="3" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1253,7 +1438,7 @@
       <c r="C51" s="6"/>
       <c r="D51" s="7"/>
       <c r="E51" s="3" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1262,7 +1447,7 @@
       <c r="C52" s="6"/>
       <c r="D52" s="7"/>
       <c r="E52" s="3" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1271,7 +1456,7 @@
       <c r="C53" s="6"/>
       <c r="D53" s="7"/>
       <c r="E53" s="3" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1280,7 +1465,7 @@
       <c r="C54" s="6"/>
       <c r="D54" s="7"/>
       <c r="E54" s="3" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1289,7 +1474,7 @@
       <c r="C55" s="6"/>
       <c r="D55" s="7"/>
       <c r="E55" s="3" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1297,28 +1482,36 @@
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
       <c r="D56" s="7"/>
-      <c r="E56" s="3"/>
+      <c r="E56" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
       <c r="D57" s="7"/>
-      <c r="E57" s="3"/>
+      <c r="E57" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
       <c r="D58" s="7"/>
-      <c r="E58" s="3"/>
+      <c r="E58" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
       <c r="D59" s="7"/>
-      <c r="E59" s="3"/>
+      <c r="E59" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
@@ -1329,21 +1522,27 @@
       <c r="D60" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E60" s="3"/>
+      <c r="E60" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
       <c r="D61" s="7"/>
-      <c r="E61" s="3"/>
+      <c r="E61" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
       <c r="D62" s="7"/>
-      <c r="E62" s="3"/>
+      <c r="E62" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
@@ -1354,21 +1553,27 @@
       </c>
       <c r="C63" s="6"/>
       <c r="D63" s="7"/>
-      <c r="E63" s="3"/>
+      <c r="E63" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
       <c r="D64" s="7"/>
-      <c r="E64" s="3"/>
+      <c r="E64" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
       <c r="D65" s="7"/>
-      <c r="E65" s="3"/>
+      <c r="E65" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
@@ -1381,21 +1586,27 @@
       <c r="D66" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E66" s="3"/>
+      <c r="E66" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
       <c r="D67" s="7"/>
-      <c r="E67" s="3"/>
+      <c r="E67" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
       <c r="D68" s="7"/>
-      <c r="E68" s="3"/>
+      <c r="E68" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
@@ -1406,21 +1617,27 @@
       </c>
       <c r="C69" s="6"/>
       <c r="D69" s="7"/>
-      <c r="E69" s="3"/>
+      <c r="E69" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
       <c r="D70" s="7"/>
-      <c r="E70" s="3"/>
+      <c r="E70" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
       <c r="D71" s="7"/>
-      <c r="E71" s="3"/>
+      <c r="E71" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
@@ -1428,7 +1645,7 @@
       <c r="C72" s="6"/>
       <c r="D72" s="7"/>
       <c r="E72" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -1436,21 +1653,27 @@
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
       <c r="D73" s="7"/>
-      <c r="E73" s="3"/>
+      <c r="E73" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
       <c r="D74" s="7"/>
-      <c r="E74" s="3"/>
+      <c r="E74" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
       <c r="D75" s="7"/>
-      <c r="E75" s="3"/>
+      <c r="E75" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
@@ -1458,7 +1681,7 @@
       <c r="C76" s="6"/>
       <c r="D76" s="7"/>
       <c r="E76" s="3" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -1467,7 +1690,7 @@
       <c r="C77" s="6"/>
       <c r="D77" s="7"/>
       <c r="E77" s="3" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -1476,7 +1699,7 @@
       <c r="C78" s="6"/>
       <c r="D78" s="7"/>
       <c r="E78" s="3" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -1485,7 +1708,7 @@
       <c r="C79" s="6"/>
       <c r="D79" s="7"/>
       <c r="E79" s="3" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -1494,7 +1717,7 @@
       <c r="C80" s="6"/>
       <c r="D80" s="7"/>
       <c r="E80" s="3" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -1503,7 +1726,7 @@
       <c r="C81" s="6"/>
       <c r="D81" s="7"/>
       <c r="E81" s="3" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -1512,7 +1735,7 @@
       <c r="C82" s="6"/>
       <c r="D82" s="7"/>
       <c r="E82" s="3" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -1521,7 +1744,7 @@
       <c r="C83" s="6"/>
       <c r="D83" s="7"/>
       <c r="E83" s="3" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -1530,7 +1753,7 @@
       <c r="C84" s="6"/>
       <c r="D84" s="7"/>
       <c r="E84" s="3" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -1538,14 +1761,18 @@
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
       <c r="D85" s="7"/>
-      <c r="E85" s="3"/>
+      <c r="E85" s="3" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
       <c r="D86" s="7"/>
-      <c r="E86" s="3"/>
+      <c r="E86" s="3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="6">
@@ -1556,7 +1783,9 @@
       <c r="D87" s="7">
         <v>11</v>
       </c>
-      <c r="E87" s="3"/>
+      <c r="E87" s="3" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="6">
@@ -1567,7 +1796,9 @@
       <c r="D88" s="7">
         <v>11</v>
       </c>
-      <c r="E88" s="3"/>
+      <c r="E88" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="6">
@@ -1578,7 +1809,9 @@
       <c r="D89" s="7">
         <v>11</v>
       </c>
-      <c r="E89" s="3"/>
+      <c r="E89" s="3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="6">
@@ -1604,7 +1837,9 @@
       <c r="D91" s="7">
         <v>11</v>
       </c>
-      <c r="E91" s="3"/>
+      <c r="E91" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
@@ -1618,7 +1853,9 @@
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
       <c r="D93" s="7"/>
-      <c r="E93" s="3"/>
+      <c r="E93" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="6"/>
@@ -1640,7 +1877,9 @@
       <c r="D95" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E95" s="3"/>
+      <c r="E95" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="6"/>
@@ -1654,7 +1893,9 @@
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
       <c r="D97" s="7"/>
-      <c r="E97" s="3"/>
+      <c r="E97" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="6"/>
@@ -1668,7 +1909,9 @@
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
       <c r="D99" s="7"/>
-      <c r="E99" s="3"/>
+      <c r="E99" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
@@ -1694,7 +1937,9 @@
       <c r="D101" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E101" s="3"/>
+      <c r="E101" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
@@ -1724,7 +1969,9 @@
       <c r="D103" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E103" s="3"/>
+      <c r="E103" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
@@ -1752,7 +1999,9 @@
         <v>1</v>
       </c>
       <c r="D105" s="7"/>
-      <c r="E105" s="3"/>
+      <c r="E105" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="6"/>
@@ -1774,7 +2023,9 @@
         <v>1</v>
       </c>
       <c r="D107" s="7"/>
-      <c r="E107" s="3"/>
+      <c r="E107" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="6"/>
@@ -1796,7 +2047,9 @@
         <v>1</v>
       </c>
       <c r="D109" s="7"/>
-      <c r="E109" s="3"/>
+      <c r="E109" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="6"/>
@@ -1810,7 +2063,9 @@
       <c r="B111" s="6"/>
       <c r="C111" s="6"/>
       <c r="D111" s="7"/>
-      <c r="E111" s="3"/>
+      <c r="E111" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="6"/>
@@ -1824,7 +2079,9 @@
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
       <c r="D113" s="7"/>
-      <c r="E113" s="3"/>
+      <c r="E113" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="6"/>
@@ -1838,7 +2095,9 @@
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
       <c r="D115" s="7"/>
-      <c r="E115" s="3"/>
+      <c r="E115" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="6"/>
@@ -1852,7 +2111,9 @@
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
       <c r="D117" s="7"/>
-      <c r="E117" s="3"/>
+      <c r="E117" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
@@ -2077,7 +2338,7 @@
       </c>
       <c r="D137" s="7"/>
       <c r="E137" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -2086,7 +2347,7 @@
       <c r="C138" s="6"/>
       <c r="D138" s="7"/>
       <c r="E138" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -2095,7 +2356,7 @@
       <c r="C139" s="6"/>
       <c r="D139" s="7"/>
       <c r="E139" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -2104,7 +2365,7 @@
       <c r="C140" s="6"/>
       <c r="D140" s="7"/>
       <c r="E140" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -2113,7 +2374,7 @@
       <c r="C141" s="6"/>
       <c r="D141" s="7"/>
       <c r="E141" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -2122,7 +2383,7 @@
       <c r="C142" s="6"/>
       <c r="D142" s="7"/>
       <c r="E142" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -2131,7 +2392,7 @@
       <c r="C143" s="6"/>
       <c r="D143" s="7"/>
       <c r="E143" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -2140,7 +2401,7 @@
       <c r="C144" s="6"/>
       <c r="D144" s="7"/>
       <c r="E144" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -2149,7 +2410,7 @@
       <c r="C145" s="6"/>
       <c r="D145" s="7"/>
       <c r="E145" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -2158,7 +2419,7 @@
       <c r="C146" s="6"/>
       <c r="D146" s="7"/>
       <c r="E146" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -2167,7 +2428,7 @@
       <c r="C147" s="6"/>
       <c r="D147" s="7"/>
       <c r="E147" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -2176,7 +2437,7 @@
       <c r="C148" s="6"/>
       <c r="D148" s="7"/>
       <c r="E148" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -2185,7 +2446,7 @@
       <c r="C149" s="6"/>
       <c r="D149" s="7"/>
       <c r="E149" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -2194,7 +2455,7 @@
       <c r="C150" s="6"/>
       <c r="D150" s="7"/>
       <c r="E150" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -2203,7 +2464,7 @@
       <c r="C151" s="6"/>
       <c r="D151" s="7"/>
       <c r="E151" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -2216,7 +2477,7 @@
       </c>
       <c r="D152" s="7"/>
       <c r="E152" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -2225,7 +2486,7 @@
       <c r="C153" s="6"/>
       <c r="D153" s="7"/>
       <c r="E153" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -2234,7 +2495,7 @@
       <c r="C154" s="6"/>
       <c r="D154" s="7"/>
       <c r="E154" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -2243,7 +2504,7 @@
       <c r="C155" s="6"/>
       <c r="D155" s="7"/>
       <c r="E155" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -2252,7 +2513,7 @@
       <c r="C156" s="6"/>
       <c r="D156" s="7"/>
       <c r="E156" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -2261,7 +2522,7 @@
       <c r="C157" s="6"/>
       <c r="D157" s="7"/>
       <c r="E157" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -2270,7 +2531,7 @@
       <c r="C158" s="6"/>
       <c r="D158" s="7"/>
       <c r="E158" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -2279,7 +2540,7 @@
       <c r="C159" s="6"/>
       <c r="D159" s="7"/>
       <c r="E159" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -2288,7 +2549,7 @@
       <c r="C160" s="6"/>
       <c r="D160" s="7"/>
       <c r="E160" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -2297,7 +2558,7 @@
       <c r="C161" s="6"/>
       <c r="D161" s="7"/>
       <c r="E161" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -2306,7 +2567,7 @@
       <c r="C162" s="6"/>
       <c r="D162" s="7"/>
       <c r="E162" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -2315,7 +2576,7 @@
       <c r="C163" s="6"/>
       <c r="D163" s="7"/>
       <c r="E163" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -2332,7 +2593,7 @@
         <v>1</v>
       </c>
       <c r="E164" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -2349,7 +2610,7 @@
         <v>1</v>
       </c>
       <c r="E165" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -2366,7 +2627,7 @@
         <v>1</v>
       </c>
       <c r="E166" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -2383,7 +2644,7 @@
         <v>30</v>
       </c>
       <c r="E167" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -2400,7 +2661,7 @@
         <v>1</v>
       </c>
       <c r="E168" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -2417,7 +2678,7 @@
         <v>1</v>
       </c>
       <c r="E169" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -2434,7 +2695,7 @@
         <v>1</v>
       </c>
       <c r="E170" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -2443,7 +2704,7 @@
       <c r="C171" s="6"/>
       <c r="D171" s="7"/>
       <c r="E171" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -2452,7 +2713,7 @@
       <c r="C172" s="6"/>
       <c r="D172" s="7"/>
       <c r="E172" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -2461,7 +2722,7 @@
       <c r="C173" s="6"/>
       <c r="D173" s="7"/>
       <c r="E173" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -2472,7 +2733,7 @@
       </c>
       <c r="D174" s="7"/>
       <c r="E174" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -2483,7 +2744,7 @@
       </c>
       <c r="D175" s="7"/>
       <c r="E175" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -2498,7 +2759,7 @@
         <v>6</v>
       </c>
       <c r="E176" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -2509,7 +2770,7 @@
       </c>
       <c r="D177" s="7"/>
       <c r="E177" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -2520,7 +2781,7 @@
       <c r="C178" s="6"/>
       <c r="D178" s="7"/>
       <c r="E178" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
@@ -2531,7 +2792,7 @@
       <c r="C179" s="6"/>
       <c r="D179" s="7"/>
       <c r="E179" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -2548,7 +2809,7 @@
         <v>10</v>
       </c>
       <c r="E180" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -2559,7 +2820,7 @@
       <c r="C181" s="6"/>
       <c r="D181" s="7"/>
       <c r="E181" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -2568,7 +2829,7 @@
       <c r="C182" s="6"/>
       <c r="D182" s="7"/>
       <c r="E182" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -2579,7 +2840,7 @@
       </c>
       <c r="D183" s="7"/>
       <c r="E183" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -2596,7 +2857,7 @@
         <v>6</v>
       </c>
       <c r="E184" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -2607,7 +2868,7 @@
       </c>
       <c r="D185" s="7"/>
       <c r="E185" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -2618,7 +2879,7 @@
       </c>
       <c r="D186" s="7"/>
       <c r="E186" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -2627,7 +2888,7 @@
       <c r="C187" s="6"/>
       <c r="D187" s="7"/>
       <c r="E187" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -2636,7 +2897,7 @@
       <c r="C188" s="6"/>
       <c r="D188" s="7"/>
       <c r="E188" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -2645,7 +2906,7 @@
       <c r="C189" s="6"/>
       <c r="D189" s="7"/>
       <c r="E189" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -2654,7 +2915,7 @@
       <c r="C190" s="6"/>
       <c r="D190" s="7"/>
       <c r="E190" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -2671,7 +2932,7 @@
         <v>0</v>
       </c>
       <c r="E191" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -2680,7 +2941,7 @@
       <c r="C192" s="6"/>
       <c r="D192" s="7"/>
       <c r="E192" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -2689,7 +2950,7 @@
       <c r="C193" s="6"/>
       <c r="D193" s="7"/>
       <c r="E193" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -2702,7 +2963,7 @@
         <v>34</v>
       </c>
       <c r="E194" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -2715,7 +2976,7 @@
         <v>1</v>
       </c>
       <c r="E195" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -2728,7 +2989,7 @@
         <v>34</v>
       </c>
       <c r="E196" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -2745,7 +3006,7 @@
         <v>34</v>
       </c>
       <c r="E197" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -2762,7 +3023,7 @@
         <v>34</v>
       </c>
       <c r="E198" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -2775,7 +3036,7 @@
       </c>
       <c r="D199" s="7"/>
       <c r="E199" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -2788,7 +3049,7 @@
       </c>
       <c r="D200" s="7"/>
       <c r="E200" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -2801,7 +3062,7 @@
       </c>
       <c r="D201" s="7"/>
       <c r="E201" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -2810,7 +3071,7 @@
       <c r="C202" s="6"/>
       <c r="D202" s="7"/>
       <c r="E202" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -2819,7 +3080,7 @@
       <c r="C203" s="6"/>
       <c r="D203" s="7"/>
       <c r="E203" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -2828,7 +3089,7 @@
       <c r="C204" s="6"/>
       <c r="D204" s="7"/>
       <c r="E204" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -2837,7 +3098,7 @@
       <c r="C205" s="6"/>
       <c r="D205" s="7"/>
       <c r="E205" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
@@ -2846,7 +3107,7 @@
       <c r="C206" s="6"/>
       <c r="D206" s="7"/>
       <c r="E206" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
@@ -2855,7 +3116,7 @@
       <c r="C207" s="6"/>
       <c r="D207" s="7"/>
       <c r="E207" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -2864,7 +3125,7 @@
       <c r="C208" s="6"/>
       <c r="D208" s="7"/>
       <c r="E208" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -2873,7 +3134,7 @@
       <c r="C209" s="6"/>
       <c r="D209" s="7"/>
       <c r="E209" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -2882,7 +3143,7 @@
       <c r="C210" s="6"/>
       <c r="D210" s="7"/>
       <c r="E210" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -2891,7 +3152,7 @@
       <c r="C211" s="6"/>
       <c r="D211" s="7"/>
       <c r="E211" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -2900,7 +3161,7 @@
       <c r="C212" s="6"/>
       <c r="D212" s="7"/>
       <c r="E212" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -2913,7 +3174,7 @@
       </c>
       <c r="D213" s="7"/>
       <c r="E213" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -2926,7 +3187,7 @@
       </c>
       <c r="D214" s="7"/>
       <c r="E214" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -2943,7 +3204,7 @@
         <v>12</v>
       </c>
       <c r="E215" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
@@ -2956,7 +3217,7 @@
       </c>
       <c r="D216" s="7"/>
       <c r="E216" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -2969,7 +3230,7 @@
       </c>
       <c r="D217" s="7"/>
       <c r="E217" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
@@ -2978,7 +3239,7 @@
       <c r="C218" s="6"/>
       <c r="D218" s="7"/>
       <c r="E218" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -2987,7 +3248,7 @@
       <c r="C219" s="6"/>
       <c r="D219" s="7"/>
       <c r="E219" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -2996,7 +3257,7 @@
       <c r="C220" s="6"/>
       <c r="D220" s="7"/>
       <c r="E220" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
@@ -3005,7 +3266,7 @@
       <c r="C221" s="6"/>
       <c r="D221" s="7"/>
       <c r="E221" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
@@ -3022,7 +3283,7 @@
         <v>14</v>
       </c>
       <c r="E222" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -3031,7 +3292,7 @@
       <c r="C223" s="6"/>
       <c r="D223" s="7"/>
       <c r="E223" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -3040,7 +3301,7 @@
       <c r="C224" s="6"/>
       <c r="D224" s="7"/>
       <c r="E224" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -3053,7 +3314,7 @@
       </c>
       <c r="D225" s="7"/>
       <c r="E225" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
@@ -3066,7 +3327,7 @@
       </c>
       <c r="D226" s="7"/>
       <c r="E226" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
@@ -3079,7 +3340,7 @@
       </c>
       <c r="D227" s="7"/>
       <c r="E227" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
@@ -3092,7 +3353,7 @@
       </c>
       <c r="D228" s="7"/>
       <c r="E228" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -3101,7 +3362,7 @@
       <c r="C229" s="6"/>
       <c r="D229" s="7"/>
       <c r="E229" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
@@ -3110,7 +3371,7 @@
       <c r="C230" s="6"/>
       <c r="D230" s="7"/>
       <c r="E230" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -3123,7 +3384,7 @@
       </c>
       <c r="D231" s="7"/>
       <c r="E231" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
@@ -3136,7 +3397,7 @@
       </c>
       <c r="D232" s="7"/>
       <c r="E232" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
@@ -3149,7 +3410,7 @@
       </c>
       <c r="D233" s="7"/>
       <c r="E233" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
@@ -3162,7 +3423,7 @@
       </c>
       <c r="D234" s="7"/>
       <c r="E234" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
@@ -3179,7 +3440,7 @@
         <v>14</v>
       </c>
       <c r="E235" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
@@ -3196,7 +3457,7 @@
         <v>14</v>
       </c>
       <c r="E236" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
@@ -3209,7 +3470,7 @@
       </c>
       <c r="D237" s="7"/>
       <c r="E237" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
@@ -3222,7 +3483,7 @@
       </c>
       <c r="D238" s="7"/>
       <c r="E238" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
@@ -3235,7 +3496,7 @@
       </c>
       <c r="D239" s="7"/>
       <c r="E239" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
@@ -3248,7 +3509,7 @@
       </c>
       <c r="D240" s="7"/>
       <c r="E240" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -3261,7 +3522,7 @@
       </c>
       <c r="D241" s="7"/>
       <c r="E241" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
@@ -3274,7 +3535,7 @@
       </c>
       <c r="D242" s="7"/>
       <c r="E242" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
@@ -3287,7 +3548,7 @@
       </c>
       <c r="D243" s="7"/>
       <c r="E243" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
@@ -3303,76 +3564,76 @@
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B245" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C245" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D245" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E245" s="3"/>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B246" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C246" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D246" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="B246" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C246" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D246" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="E246" s="3"/>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B247" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C247" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D247" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="C247" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D247" s="7" t="s">
-        <v>53</v>
       </c>
       <c r="E247" s="3"/>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B248" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C248" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D248" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="B248" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C248" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D248" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="E248" s="3"/>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B249" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C249" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D249" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E249" s="3"/>
     </row>
@@ -4143,18 +4404,14 @@
       <c r="B332" s="6"/>
       <c r="C332" s="6"/>
       <c r="D332" s="7"/>
-      <c r="E332" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="E332" s="3"/>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="6"/>
       <c r="B333" s="6"/>
       <c r="C333" s="6"/>
       <c r="D333" s="7"/>
-      <c r="E333" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="E333" s="3"/>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="6">
@@ -4163,9 +4420,7 @@
       <c r="B334" s="6"/>
       <c r="C334" s="6"/>
       <c r="D334" s="7"/>
-      <c r="E334" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="E334" s="3"/>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="6">
@@ -4174,9 +4429,7 @@
       <c r="B335" s="6"/>
       <c r="C335" s="6"/>
       <c r="D335" s="7"/>
-      <c r="E335" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="E335" s="3"/>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="6">
@@ -4185,9 +4438,7 @@
       <c r="B336" s="6"/>
       <c r="C336" s="6"/>
       <c r="D336" s="7"/>
-      <c r="E336" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="E336" s="3"/>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" s="6">
@@ -4196,9 +4447,7 @@
       <c r="B337" s="6"/>
       <c r="C337" s="6"/>
       <c r="D337" s="7"/>
-      <c r="E337" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="E337" s="3"/>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="6">
@@ -4213,27 +4462,21 @@
       <c r="D338" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E338" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="E338" s="3"/>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="6"/>
       <c r="B339" s="6"/>
       <c r="C339" s="6"/>
       <c r="D339" s="7"/>
-      <c r="E339" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="E339" s="3"/>
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="6"/>
       <c r="B340" s="6"/>
       <c r="C340" s="6"/>
       <c r="D340" s="7"/>
-      <c r="E340" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="E340" s="3"/>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="6"/>
@@ -4703,76 +4946,76 @@
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A393" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B393" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C393" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B393" s="6" t="s">
+      <c r="D393" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="C393" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D393" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="E393" s="3"/>
     </row>
     <row r="394" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A394" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B394" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C394" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D394" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E394" s="3"/>
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A395" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B395" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C395" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D395" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E395" s="3"/>
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A396" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B396" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C396" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D396" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E396" s="3"/>
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A397" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B397" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C397" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B397" s="6" t="s">
+      <c r="D397" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="C397" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D397" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="E397" s="3"/>
     </row>
@@ -4889,10 +5132,10 @@
         <v>1</v>
       </c>
       <c r="B406" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C406" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D406" s="6" t="s">
         <v>1</v>
@@ -4904,10 +5147,10 @@
         <v>1</v>
       </c>
       <c r="B407" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C407" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D407" s="6" t="s">
         <v>1</v>
@@ -4919,10 +5162,10 @@
         <v>1</v>
       </c>
       <c r="B408" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C408" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D408" s="6" t="s">
         <v>1</v>
@@ -4934,10 +5177,10 @@
         <v>1</v>
       </c>
       <c r="B409" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C409" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D409" s="6" t="s">
         <v>1</v>
@@ -4949,10 +5192,10 @@
         <v>1</v>
       </c>
       <c r="B410" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C410" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D410" s="6" t="s">
         <v>1</v>
@@ -5021,16 +5264,16 @@
     </row>
     <row r="415" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A415" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B415" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B415" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="C415" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D415" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E415" s="3"/>
     </row>
@@ -5216,16 +5459,16 @@
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A428" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B428" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B428" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="C428" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D428" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E428" s="3"/>
     </row>
@@ -5352,81 +5595,101 @@
     </row>
     <row r="440" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A440" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B440" s="6"/>
       <c r="C440" s="6"/>
       <c r="D440" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E440" s="3"/>
     </row>
     <row r="441" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A441" s="6">
-        <v>11</v>
+      <c r="A441" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="B441" s="6"/>
       <c r="C441" s="6"/>
-      <c r="D441" s="7">
-        <v>11</v>
+      <c r="D441" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="E441" s="3"/>
     </row>
     <row r="442" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A442" s="6">
-        <v>11</v>
+      <c r="A442" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="B442" s="6"/>
       <c r="C442" s="6"/>
-      <c r="D442" s="7">
-        <v>11</v>
+      <c r="D442" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="E442" s="3"/>
     </row>
     <row r="443" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A443" s="6">
-        <v>11</v>
+      <c r="A443" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="B443" s="6"/>
       <c r="C443" s="6"/>
-      <c r="D443" s="7">
-        <v>11</v>
+      <c r="D443" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="E443" s="3"/>
     </row>
     <row r="444" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A444" s="6"/>
+      <c r="A444" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="B444" s="6"/>
       <c r="C444" s="6"/>
-      <c r="D444" s="7"/>
+      <c r="D444" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="E444" s="3"/>
     </row>
     <row r="445" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A445" s="6"/>
+      <c r="A445" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="B445" s="6"/>
       <c r="C445" s="6"/>
-      <c r="D445" s="7"/>
+      <c r="D445" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="E445" s="3"/>
     </row>
     <row r="446" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A446" s="6"/>
+      <c r="A446" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="B446" s="6"/>
       <c r="C446" s="6"/>
-      <c r="D446" s="7"/>
+      <c r="D446" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="E446" s="3"/>
     </row>
     <row r="447" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A447" s="6"/>
+      <c r="A447" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="B447" s="6"/>
       <c r="C447" s="6"/>
-      <c r="D447" s="7"/>
+      <c r="D447" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="E447" s="3"/>
     </row>
     <row r="448" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A448" s="6"/>
+      <c r="A448" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="B448" s="6"/>
       <c r="C448" s="6"/>
-      <c r="D448" s="7"/>
+      <c r="D448" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="E448" s="3"/>
     </row>
     <row r="449" spans="1:5" x14ac:dyDescent="0.25">
@@ -5533,8 +5796,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="G1:Q1"/>
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="G10:M10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5543,6 +5806,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Лист2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5555,6 +5819,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Лист3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>